<commit_message>
Table 3- corrected a few typos
</commit_message>
<xml_diff>
--- a/manuscript/tables_figures/Table3.xlsx
+++ b/manuscript/tables_figures/Table3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kteixeira/Dropbox (Smithsonian)/GitHub/SCBI-ForestGEO/McGregor_climate-sensitivity-variation/manuscript/tables_figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6484A8-F146-BE4B-8A3A-0F0846DB4BB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52BD4EC-E1CD-E141-93FA-F825FD4127EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{CEAF6856-360D-489D-958B-5830D64CE7C9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" xr2:uid="{CEAF6856-360D-489D-958B-5830D64CE7C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>dAICc</t>
   </si>
@@ -111,10 +111,13 @@
     <t>diffuse</t>
   </si>
   <si>
-    <t>al years</t>
-  </si>
-  <si>
     <t xml:space="preserve">drought year </t>
+  </si>
+  <si>
+    <t>1964-66</t>
+  </si>
+  <si>
+    <t>all droughts</t>
   </si>
 </sst>
 </file>
@@ -223,9 +226,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -240,6 +240,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -559,7 +562,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -586,89 +589,89 @@
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
-      <c r="E2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="9">
-        <v>1964</v>
-      </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="9">
+      <c r="E2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="15"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="15">
         <v>1977</v>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="9">
+      <c r="L2" s="15"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="15">
         <v>1999</v>
       </c>
-      <c r="O2" s="9"/>
+      <c r="O2" s="15"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="11" t="s">
+      <c r="E3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="11" t="s">
+      <c r="G3" s="10"/>
+      <c r="H3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="L3" s="11" t="s">
+      <c r="J3" s="10"/>
+      <c r="K3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="O3" s="11" t="s">
+      <c r="M3" s="10"/>
+      <c r="N3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="3">
-        <v>1966</v>
-      </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>35.834000000000003</v>
       </c>
-      <c r="F4" s="12">
-        <v>0</v>
-      </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
+      <c r="F4" s="11">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
     </row>
     <row r="5" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
@@ -677,19 +680,19 @@
         <v>1977</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11">
         <v>-0.09</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
     </row>
     <row r="6" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
@@ -698,19 +701,19 @@
         <v>1999</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11">
         <v>-8.1000000000000003E-2</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
     </row>
     <row r="7" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
@@ -721,31 +724,31 @@
       <c r="D7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>7.4109999999999996</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>-3.5000000000000003E-2</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13">
+      <c r="G7" s="12"/>
+      <c r="H7" s="12">
         <v>18.276</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="12">
         <v>-8.2000000000000003E-2</v>
       </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13">
+      <c r="J7" s="12"/>
+      <c r="K7" s="12">
         <v>-0.94699999999999995</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="12">
         <v>-2.1000000000000001E-2</v>
       </c>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13">
+      <c r="M7" s="12"/>
+      <c r="N7" s="12">
         <v>-1.9179999999999999</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="12">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
@@ -758,31 +761,31 @@
       <c r="D8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>7.5910000000000002</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="11">
         <v>-5.8000000000000003E-2</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12">
+      <c r="G8" s="11"/>
+      <c r="H8" s="11">
         <v>17.788</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="11">
         <v>-0.13300000000000001</v>
       </c>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12">
+      <c r="J8" s="11"/>
+      <c r="K8" s="11">
         <v>-1.077</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="11">
         <v>-3.2000000000000001E-2</v>
       </c>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12">
+      <c r="M8" s="11"/>
+      <c r="N8" s="11">
         <v>-2.0219999999999998</v>
       </c>
-      <c r="O8" s="12">
+      <c r="O8" s="11">
         <v>2E-3</v>
       </c>
     </row>
@@ -797,31 +800,31 @@
       <c r="D9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <v>-1.46</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="12">
         <v>-5.1999999999999998E-2</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13">
+      <c r="G9" s="12"/>
+      <c r="H9" s="12">
         <v>4.4870000000000001</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="12">
         <v>-6.7000000000000004E-2</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13">
+      <c r="J9" s="12"/>
+      <c r="K9" s="12">
         <v>0.15</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="12">
         <v>-7.8E-2</v>
       </c>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13">
+      <c r="M9" s="12"/>
+      <c r="N9" s="12">
         <v>0.44400000000000001</v>
       </c>
-      <c r="O9" s="13">
+      <c r="O9" s="12">
         <v>-1.0999999999999999E-2</v>
       </c>
     </row>
@@ -834,23 +837,23 @@
         <v>8</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13">
-        <v>0</v>
-      </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13">
-        <v>0</v>
-      </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13">
-        <v>0</v>
-      </c>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13">
+      <c r="E10" s="12"/>
+      <c r="F10" s="12">
+        <v>0</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12">
+        <v>0</v>
+      </c>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12">
+        <v>0</v>
+      </c>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12">
         <v>0</v>
       </c>
     </row>
@@ -861,23 +864,23 @@
         <v>9</v>
       </c>
       <c r="D11" s="5"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13">
+      <c r="E11" s="12"/>
+      <c r="F11" s="12">
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13">
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13">
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12">
         <v>-2.8000000000000001E-2</v>
       </c>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13">
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12">
         <v>-5.6000000000000001E-2</v>
       </c>
     </row>
@@ -888,23 +891,23 @@
         <v>10</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13">
+      <c r="E12" s="12"/>
+      <c r="F12" s="12">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13">
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13">
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12">
         <v>0.04</v>
       </c>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13">
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12">
         <v>-4.9000000000000002E-2</v>
       </c>
     </row>
@@ -919,31 +922,31 @@
       <c r="D13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="11">
         <v>1.6819999999999999</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="11">
         <v>-4.3999999999999997E-2</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12">
+      <c r="G13" s="11"/>
+      <c r="H13" s="11">
         <v>-2.548</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="11">
         <v>-5.5E-2</v>
       </c>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12">
+      <c r="J13" s="11"/>
+      <c r="K13" s="11">
         <v>-0.7</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="11">
         <v>-7.5999999999999998E-2</v>
       </c>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12">
+      <c r="M13" s="11"/>
+      <c r="N13" s="11">
         <v>4.0869999999999997</v>
       </c>
-      <c r="O13" s="12">
+      <c r="O13" s="11">
         <v>-3.0000000000000001E-3</v>
       </c>
     </row>
@@ -956,23 +959,23 @@
         <v>8</v>
       </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12">
-        <v>0</v>
-      </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12">
-        <v>0</v>
-      </c>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12">
-        <v>0</v>
-      </c>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11">
+        <v>0</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11">
+        <v>0</v>
+      </c>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11">
+        <v>0</v>
+      </c>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11">
         <v>0</v>
       </c>
     </row>
@@ -983,23 +986,23 @@
         <v>9</v>
       </c>
       <c r="D15" s="3"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12">
+      <c r="E15" s="11"/>
+      <c r="F15" s="11">
         <v>-4.2000000000000003E-2</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12">
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12">
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11">
         <v>-3.3000000000000002E-2</v>
       </c>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="14">
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="13">
         <v>-8.2000000000000003E-2</v>
       </c>
     </row>
@@ -1010,23 +1013,23 @@
         <v>10</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12">
+      <c r="E16" s="11"/>
+      <c r="F16" s="11">
         <v>-5.2999999999999999E-2</v>
       </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12">
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11">
         <v>-4.3999999999999997E-2</v>
       </c>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12">
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12">
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11">
         <v>-0.10199999999999999</v>
       </c>
     </row>
@@ -1039,31 +1042,31 @@
       <c r="D17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="12">
         <v>2.88</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="12">
         <v>-6.8000000000000005E-2</v>
       </c>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13">
+      <c r="G17" s="12"/>
+      <c r="H17" s="12">
         <v>-1.2809999999999999</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I17" s="12">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13">
+      <c r="J17" s="12"/>
+      <c r="K17" s="12">
         <v>4.7279999999999998</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="12">
         <v>-0.13800000000000001</v>
       </c>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13">
+      <c r="M17" s="12"/>
+      <c r="N17" s="12">
         <v>2.621</v>
       </c>
-      <c r="O17" s="13">
+      <c r="O17" s="12">
         <v>-0.10100000000000001</v>
       </c>
     </row>
@@ -1076,31 +1079,31 @@
       <c r="D18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="13">
         <v>-2.0179999999999998</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="11">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12">
+      <c r="G18" s="11"/>
+      <c r="H18" s="11">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="11">
         <v>-0.17399999999999999</v>
       </c>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12">
+      <c r="J18" s="11"/>
+      <c r="K18" s="11">
         <v>-1.7669999999999999</v>
       </c>
-      <c r="L18" s="12">
+      <c r="L18" s="11">
         <v>0.06</v>
       </c>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12">
+      <c r="M18" s="11"/>
+      <c r="N18" s="11">
         <v>-1.7849999999999999</v>
       </c>
-      <c r="O18" s="12">
+      <c r="O18" s="11">
         <v>5.7000000000000002E-2</v>
       </c>
     </row>
@@ -1113,31 +1116,31 @@
       <c r="D19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="12">
         <v>-2.0179999999999998</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="12">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13">
+      <c r="G19" s="12"/>
+      <c r="H19" s="12">
         <v>-1.96</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="12">
         <v>-4.9000000000000002E-2</v>
       </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13">
+      <c r="J19" s="12"/>
+      <c r="K19" s="12">
         <v>-1.236</v>
       </c>
-      <c r="L19" s="13">
+      <c r="L19" s="12">
         <v>-0.17499999999999999</v>
       </c>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13">
+      <c r="M19" s="12"/>
+      <c r="N19" s="12">
         <v>0.17100000000000001</v>
       </c>
-      <c r="O19" s="13">
+      <c r="O19" s="12">
         <v>0.247</v>
       </c>
     </row>
@@ -1150,31 +1153,31 @@
       <c r="D20" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="11">
         <v>-1.895</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="11">
         <v>1E-3</v>
       </c>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12">
+      <c r="G20" s="11"/>
+      <c r="H20" s="11">
         <v>-1.075</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="11">
         <v>2E-3</v>
       </c>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12">
+      <c r="J20" s="11"/>
+      <c r="K20" s="11">
         <v>-1.698</v>
       </c>
-      <c r="L20" s="12">
+      <c r="L20" s="11">
         <v>-1E-3</v>
       </c>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12">
+      <c r="M20" s="11"/>
+      <c r="N20" s="11">
         <v>-1.9850000000000001</v>
       </c>
-      <c r="O20" s="12">
+      <c r="O20" s="11">
         <v>1E-4</v>
       </c>
     </row>
@@ -1189,31 +1192,31 @@
       <c r="D21" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="12">
         <v>-3.5529999999999999</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="12">
         <v>0.04</v>
       </c>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13">
+      <c r="G21" s="12"/>
+      <c r="H21" s="12">
         <v>-2.161</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="12">
         <v>0.10100000000000001</v>
       </c>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13">
+      <c r="J21" s="12"/>
+      <c r="K21" s="12">
         <v>0.89500000000000002</v>
       </c>
-      <c r="L21" s="13">
+      <c r="L21" s="12">
         <v>-0.19</v>
       </c>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13">
+      <c r="M21" s="12"/>
+      <c r="N21" s="12">
         <v>4.0830000000000002</v>
       </c>
-      <c r="O21" s="13">
+      <c r="O21" s="12">
         <v>0.2</v>
       </c>
     </row>
@@ -1224,23 +1227,23 @@
         <v>12</v>
       </c>
       <c r="D22" s="5"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13">
+      <c r="E22" s="12"/>
+      <c r="F22" s="12">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13">
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13">
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12">
         <v>-0.14699999999999999</v>
       </c>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13">
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12">
         <v>0.151</v>
       </c>
     </row>
@@ -1251,25 +1254,25 @@
         <v>27</v>
       </c>
       <c r="D23" s="5"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13">
-        <v>0</v>
-      </c>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13">
-        <v>0</v>
-      </c>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13">
-        <v>0</v>
-      </c>
-      <c r="L23" s="13">
-        <v>0</v>
-      </c>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13">
+      <c r="E23" s="12"/>
+      <c r="F23" s="12">
+        <v>0</v>
+      </c>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12">
+        <v>0</v>
+      </c>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12">
+        <v>0</v>
+      </c>
+      <c r="L23" s="12">
+        <v>0</v>
+      </c>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12">
         <v>0</v>
       </c>
     </row>
@@ -1282,31 +1285,31 @@
       <c r="D24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="11">
         <v>4.58</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="11">
         <v>-0.20699999999999999</v>
       </c>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12">
+      <c r="G24" s="11"/>
+      <c r="H24" s="11">
         <v>1.3520000000000001</v>
       </c>
-      <c r="I24" s="12">
+      <c r="I24" s="11">
         <v>-0.217</v>
       </c>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12">
+      <c r="J24" s="11"/>
+      <c r="K24" s="11">
         <v>1.008</v>
       </c>
-      <c r="L24" s="12">
+      <c r="L24" s="11">
         <v>-0.23599999999999999</v>
       </c>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12">
+      <c r="M24" s="11"/>
+      <c r="N24" s="11">
         <v>0.13200000000000001</v>
       </c>
-      <c r="O24" s="12">
+      <c r="O24" s="11">
         <v>-0.17699999999999999</v>
       </c>
     </row>
@@ -1319,31 +1322,31 @@
       <c r="D25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="14">
         <v>4.4130000000000003</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="14">
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15">
+      <c r="G25" s="14"/>
+      <c r="H25" s="14">
         <v>5.8250000000000002</v>
       </c>
-      <c r="I25" s="15">
+      <c r="I25" s="14">
         <v>-1.6E-2</v>
       </c>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15">
+      <c r="J25" s="14"/>
+      <c r="K25" s="14">
         <v>-0.19</v>
       </c>
-      <c r="L25" s="15">
+      <c r="L25" s="14">
         <v>-0.01</v>
       </c>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15">
+      <c r="M25" s="14"/>
+      <c r="N25" s="14">
         <v>-0.70099999999999996</v>
       </c>
-      <c r="O25" s="15">
+      <c r="O25" s="14">
         <v>-7.0000000000000001E-3</v>
       </c>
     </row>

</xml_diff>